<commit_message>
update to new format inv
</commit_message>
<xml_diff>
--- a/public/sampleAP.xlsx
+++ b/public/sampleAP.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp_8\htdocs\coba_newitportal\IT-PORTAL-HO\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp_8\htdocs\new\IT-PORTAL-HO\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B188C76-6276-46EA-BF53-514832295F03}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CCF2BEC-E5A2-4AAC-914A-1092B0B1C92E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AA518A1B-D065-49A0-8AFF-0FB34B05899E}"/>
   </bookViews>
@@ -138,7 +138,7 @@
     <t>PPAHOAP003</t>
   </si>
   <si>
-    <t>PPAHOAP004</t>
+    <t>PPAHOAP001</t>
   </si>
 </sst>
 </file>
@@ -675,20 +675,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="6.69921875" customWidth="1"/>
-    <col min="2" max="2" width="13.296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.3984375" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.8984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.3984375" customWidth="1"/>
-    <col min="7" max="7" width="34.3984375" customWidth="1"/>
-    <col min="8" max="8" width="14.8984375" customWidth="1"/>
-    <col min="9" max="9" width="17.8984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.37890625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.90234375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.47265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.37890625" customWidth="1"/>
+    <col min="7" max="7" width="34.37890625" customWidth="1"/>
+    <col min="8" max="8" width="14.90234375" customWidth="1"/>
+    <col min="9" max="9" width="17.90234375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="28" customWidth="1"/>
-    <col min="11" max="11" width="16.69921875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.296875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="30.19921875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="30.1875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1">
@@ -923,7 +923,7 @@
       <c r="M15" s="8"/>
       <c r="N15" s="8"/>
     </row>
-    <row r="16" spans="1:14" ht="26.4">
+    <row r="16" spans="1:14" ht="24.6">
       <c r="A16" s="1" t="s">
         <v>33</v>
       </c>
@@ -978,7 +978,7 @@
         <v>123</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>12</v>
@@ -1022,7 +1022,7 @@
         <v>1234</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>22</v>
@@ -1066,7 +1066,7 @@
         <v>12345</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>28</v>

</xml_diff>